<commit_message>
Agile Project Intro 1st week
</commit_message>
<xml_diff>
--- a/Agile Project Intro.xlsx
+++ b/Agile Project Intro.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -159,6 +159,21 @@
   </si>
   <si>
     <t>TOTAL TIME</t>
+  </si>
+  <si>
+    <t>Group Members</t>
+  </si>
+  <si>
+    <t>Nazlı Karalar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gamze Küçükçolak </t>
+  </si>
+  <si>
+    <t>Mehmet Kağan Kayaalp</t>
+  </si>
+  <si>
+    <t>Erdi Koç</t>
   </si>
 </sst>
 </file>
@@ -197,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +237,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -264,11 +285,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -283,9 +356,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,6 +368,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,11 +511,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101171200"/>
-        <c:axId val="101172736"/>
+        <c:axId val="200542464"/>
+        <c:axId val="200544256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101171200"/>
+        <c:axId val="200542464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101172736"/>
+        <c:crossAx val="200544256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -465,7 +542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101172736"/>
+        <c:axId val="200544256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -477,7 +554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101171200"/>
+        <c:crossAx val="200542464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -816,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S16"/>
+  <dimension ref="B2:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,26 +910,28 @@
     <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+    <row r="2" spans="2:22" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="4"/>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,29 +981,35 @@
       <c r="S3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="U3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="14">
-        <v>5</v>
-      </c>
-      <c r="E4" s="14">
+      <c r="D4" s="13">
+        <v>5</v>
+      </c>
+      <c r="E4" s="13">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <f>E4</f>
         <v>3</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <f>0</f>
         <v>0</v>
       </c>
@@ -941,35 +1026,38 @@
       <c r="Q4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="13">
         <v>3</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="V4" s="18" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14">
-        <v>5</v>
-      </c>
-      <c r="E5" s="14">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="13">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13">
+        <v>5</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <f t="shared" ref="H5:H15" si="0">E5</f>
         <v>5</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <f>0</f>
         <v>0</v>
       </c>
@@ -986,35 +1074,38 @@
       <c r="Q5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="14">
-        <v>5</v>
-      </c>
-      <c r="S5" s="11" t="s">
+      <c r="R5" s="13">
+        <v>5</v>
+      </c>
+      <c r="S5" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="V5" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <f>E6</f>
         <v>4</v>
       </c>
@@ -1025,33 +1116,36 @@
       <c r="Q6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R6" s="16">
+      <c r="R6" s="15">
         <f>SUM(R4:R5)</f>
         <v>8</v>
       </c>
+      <c r="V6" s="18" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>8</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <f t="shared" ref="I7:I15" si="1">E7</f>
         <v>8</v>
       </c>
@@ -1059,29 +1153,32 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
+      <c r="V7" s="19" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>2</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>6</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1090,28 +1187,28 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>4</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>8</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -1120,28 +1217,28 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="14">
-        <v>5</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="13">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
         <v>4</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1150,28 +1247,28 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="14">
-        <v>5</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="13">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1180,28 +1277,28 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="14">
-        <v>5</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="13">
+        <v>5</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1210,28 +1307,28 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>3</v>
       </c>
-      <c r="E13" s="14">
-        <v>5</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="E13" s="13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1240,28 +1337,28 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>3</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>8</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -1270,28 +1367,28 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>2</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <v>3</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="14">
+      <c r="H15" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1300,7 +1397,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>46</v>
       </c>

</xml_diff>